<commit_message>
30 min cat only 2
3 spd, 8 sight, 7 time
</commit_message>
<xml_diff>
--- a/Mixed Logs.xlsx
+++ b/Mixed Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Chicken, cat, dog\Dog-Cat_Chicken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABDF4A2-A2AA-4A8A-9FFF-F0B9D5F2311D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB309C4-7985-417F-A38B-614E808032FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E5509BF1-11B8-46C2-87AA-D7FA4F3627F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="1445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="1703">
   <si>
     <t>1 hour simulation</t>
   </si>
@@ -4371,6 +4371,780 @@
   </si>
   <si>
     <t>[5/4/2025 7:24:04 PM]Simulation Counter : 273, Last winner cat had: 20 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>30 min cat only, 3spd, 8 sight, 7 time</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:17:44 PM]Simulation Counter : 0, Last winner cat had: 20 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:17:51 PM]Simulation Counter : 1, Last winner cat had: 12 points! Last winner dog had: 20.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:17:58 PM]Simulation Counter : 2, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:05 PM]Simulation Counter : 3, Last winner cat had: 14 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:12 PM]Simulation Counter : 4, Last winner cat had: 12 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:19 PM]Simulation Counter : 5, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:26 PM]Simulation Counter : 6, Last winner cat had: 14 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:33 PM]Simulation Counter : 7, Last winner cat had: 14 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:40 PM]Simulation Counter : 8, Last winner cat had: 12 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:47 PM]Simulation Counter : 9, Last winner cat had: 14 points! Last winner dog had: 11 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:18:54 PM]Simulation Counter : 10, Last winner cat had: 12 points! Last winner dog had: 10.9 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:01 PM]Simulation Counter : 11, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:08 PM]Simulation Counter : 12, Last winner cat had: 12 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:15 PM]Simulation Counter : 13, Last winner cat had: 14 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:22 PM]Simulation Counter : 14, Last winner cat had: 12 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:29 PM]Simulation Counter : 15, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:36 PM]Simulation Counter : 16, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:43 PM]Simulation Counter : 17, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:50 PM]Simulation Counter : 18, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:19:57 PM]Simulation Counter : 19, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:04 PM]Simulation Counter : 20, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:11 PM]Simulation Counter : 21, Last winner cat had: 12 points! Last winner dog had: 20 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:18 PM]Simulation Counter : 22, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:25 PM]Simulation Counter : 23, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:32 PM]Simulation Counter : 24, Last winner cat had: 12 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:39 PM]Simulation Counter : 25, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:46 PM]Simulation Counter : 26, Last winner cat had: 12 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:20:53 PM]Simulation Counter : 27, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:00 PM]Simulation Counter : 28, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:07 PM]Simulation Counter : 29, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:14 PM]Simulation Counter : 30, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:21 PM]Simulation Counter : 31, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:28 PM]Simulation Counter : 32, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:35 PM]Simulation Counter : 33, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:42 PM]Simulation Counter : 34, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:49 PM]Simulation Counter : 35, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:21:56 PM]Simulation Counter : 36, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:03 PM]Simulation Counter : 37, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:10 PM]Simulation Counter : 38, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:17 PM]Simulation Counter : 39, Last winner cat had: 12 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:24 PM]Simulation Counter : 40, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:31 PM]Simulation Counter : 41, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:38 PM]Simulation Counter : 42, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:45 PM]Simulation Counter : 43, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:52 PM]Simulation Counter : 44, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:22:59 PM]Simulation Counter : 45, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:06 PM]Simulation Counter : 46, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:13 PM]Simulation Counter : 47, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:20 PM]Simulation Counter : 48, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:27 PM]Simulation Counter : 49, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:34 PM]Simulation Counter : 50, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:41 PM]Simulation Counter : 51, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:48 PM]Simulation Counter : 52, Last winner cat had: 10 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:23:55 PM]Simulation Counter : 53, Last winner cat had: 10 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:02 PM]Simulation Counter : 54, Last winner cat had: 10 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:09 PM]Simulation Counter : 55, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:16 PM]Simulation Counter : 56, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:23 PM]Simulation Counter : 57, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:30 PM]Simulation Counter : 58, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:37 PM]Simulation Counter : 59, Last winner cat had: 10 points! Last winner dog had: 10.5 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:44 PM]Simulation Counter : 60, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:51 PM]Simulation Counter : 61, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:24:58 PM]Simulation Counter : 62, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:05 PM]Simulation Counter : 63, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:12 PM]Simulation Counter : 64, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:19 PM]Simulation Counter : 65, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:26 PM]Simulation Counter : 66, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:33 PM]Simulation Counter : 67, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:40 PM]Simulation Counter : 68, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:47 PM]Simulation Counter : 69, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:25:54 PM]Simulation Counter : 70, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:01 PM]Simulation Counter : 71, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:08 PM]Simulation Counter : 72, Last winner cat had: 12 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:15 PM]Simulation Counter : 73, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:22 PM]Simulation Counter : 74, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:29 PM]Simulation Counter : 75, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:36 PM]Simulation Counter : 76, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:43 PM]Simulation Counter : 77, Last winner cat had: 10 points! Last winner dog had: 10.5 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:50 PM]Simulation Counter : 78, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:26:57 PM]Simulation Counter : 79, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:04 PM]Simulation Counter : 80, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:11 PM]Simulation Counter : 81, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:18 PM]Simulation Counter : 82, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:25 PM]Simulation Counter : 83, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:32 PM]Simulation Counter : 84, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:39 PM]Simulation Counter : 85, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:46 PM]Simulation Counter : 86, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:27:53 PM]Simulation Counter : 87, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:00 PM]Simulation Counter : 88, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:07 PM]Simulation Counter : 89, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:14 PM]Simulation Counter : 90, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:21 PM]Simulation Counter : 91, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:28 PM]Simulation Counter : 92, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:35 PM]Simulation Counter : 93, Last winner cat had: 12 points! Last winner dog had: 20.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:42 PM]Simulation Counter : 94, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:49 PM]Simulation Counter : 95, Last winner cat had: 10 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:28:56 PM]Simulation Counter : 96, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:03 PM]Simulation Counter : 97, Last winner cat had: 12 points! Last winner dog had: 10.6 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:10 PM]Simulation Counter : 98, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:17 PM]Simulation Counter : 99, Last winner cat had: 12 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:24 PM]Simulation Counter : 100, Last winner cat had: 12 points! Last winner dog had: 10.5 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:31 PM]Simulation Counter : 101, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:38 PM]Simulation Counter : 102, Last winner cat had: 14 points! Last winner dog had: 10.6 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:45 PM]Simulation Counter : 103, Last winner cat had: 12 points! Last winner dog had: 20 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:52 PM]Simulation Counter : 104, Last winner cat had: 12 points! Last winner dog had: 20.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:29:59 PM]Simulation Counter : 105, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:06 PM]Simulation Counter : 106, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:13 PM]Simulation Counter : 107, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:20 PM]Simulation Counter : 108, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:27 PM]Simulation Counter : 109, Last winner cat had: 12 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:34 PM]Simulation Counter : 110, Last winner cat had: 10 points! Last winner dog had: 20.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:41 PM]Simulation Counter : 111, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:48 PM]Simulation Counter : 112, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:30:55 PM]Simulation Counter : 113, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:02 PM]Simulation Counter : 114, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:09 PM]Simulation Counter : 115, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:16 PM]Simulation Counter : 116, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:23 PM]Simulation Counter : 117, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:30 PM]Simulation Counter : 118, Last winner cat had: 12 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:37 PM]Simulation Counter : 119, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:44 PM]Simulation Counter : 120, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:51 PM]Simulation Counter : 121, Last winner cat had: 10 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:31:58 PM]Simulation Counter : 122, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:05 PM]Simulation Counter : 123, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:12 PM]Simulation Counter : 124, Last winner cat had: 12 points! Last winner dog had: 10.5 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:19 PM]Simulation Counter : 125, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:26 PM]Simulation Counter : 126, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:33 PM]Simulation Counter : 127, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:40 PM]Simulation Counter : 128, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:47 PM]Simulation Counter : 129, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:32:54 PM]Simulation Counter : 130, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:01 PM]Simulation Counter : 131, Last winner cat had: 10 points! Last winner dog had: 10.5 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:08 PM]Simulation Counter : 132, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:15 PM]Simulation Counter : 133, Last winner cat had: 10 points! Last winner dog had: 20.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:22 PM]Simulation Counter : 134, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:29 PM]Simulation Counter : 135, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:36 PM]Simulation Counter : 136, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:43 PM]Simulation Counter : 137, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:50 PM]Simulation Counter : 138, Last winner cat had: 10 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:33:57 PM]Simulation Counter : 139, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:04 PM]Simulation Counter : 140, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:11 PM]Simulation Counter : 141, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:18 PM]Simulation Counter : 142, Last winner cat had: 12 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:25 PM]Simulation Counter : 143, Last winner cat had: 12 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:32 PM]Simulation Counter : 144, Last winner cat had: 12 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:39 PM]Simulation Counter : 145, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:46 PM]Simulation Counter : 146, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:34:53 PM]Simulation Counter : 147, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:00 PM]Simulation Counter : 148, Last winner cat had: 12 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:07 PM]Simulation Counter : 149, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:14 PM]Simulation Counter : 150, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:21 PM]Simulation Counter : 151, Last winner cat had: 12 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:28 PM]Simulation Counter : 152, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:35 PM]Simulation Counter : 153, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:42 PM]Simulation Counter : 154, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:49 PM]Simulation Counter : 155, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:35:56 PM]Simulation Counter : 156, Last winner cat had: 10 points! Last winner dog had: 20.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:03 PM]Simulation Counter : 157, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:10 PM]Simulation Counter : 158, Last winner cat had: 10 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:17 PM]Simulation Counter : 159, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:24 PM]Simulation Counter : 160, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:31 PM]Simulation Counter : 161, Last winner cat had: 12 points! Last winner dog had: 20 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:38 PM]Simulation Counter : 162, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:45 PM]Simulation Counter : 163, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:52 PM]Simulation Counter : 164, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:36:59 PM]Simulation Counter : 165, Last winner cat had: 10 points! Last winner dog had: 20 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:06 PM]Simulation Counter : 166, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:13 PM]Simulation Counter : 167, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:20 PM]Simulation Counter : 168, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:27 PM]Simulation Counter : 169, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:34 PM]Simulation Counter : 170, Last winner cat had: 10 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:41 PM]Simulation Counter : 171, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:48 PM]Simulation Counter : 172, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:37:55 PM]Simulation Counter : 173, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:02 PM]Simulation Counter : 174, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:09 PM]Simulation Counter : 175, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:16 PM]Simulation Counter : 176, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:23 PM]Simulation Counter : 177, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:30 PM]Simulation Counter : 178, Last winner cat had: 12 points! Last winner dog had: 20 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:37 PM]Simulation Counter : 179, Last winner cat had: 10 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:44 PM]Simulation Counter : 180, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:51 PM]Simulation Counter : 181, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:38:58 PM]Simulation Counter : 182, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:05 PM]Simulation Counter : 183, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:12 PM]Simulation Counter : 184, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:19 PM]Simulation Counter : 185, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:26 PM]Simulation Counter : 186, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:33 PM]Simulation Counter : 187, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:40 PM]Simulation Counter : 188, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:47 PM]Simulation Counter : 189, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:39:54 PM]Simulation Counter : 190, Last winner cat had: 14 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:01 PM]Simulation Counter : 191, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:08 PM]Simulation Counter : 192, Last winner cat had: 12 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:15 PM]Simulation Counter : 193, Last winner cat had: 12 points! Last winner dog had: 20.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:22 PM]Simulation Counter : 194, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:29 PM]Simulation Counter : 195, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:36 PM]Simulation Counter : 196, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:43 PM]Simulation Counter : 197, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:50 PM]Simulation Counter : 198, Last winner cat had: 10 points! Last winner dog had: 15.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:40:57 PM]Simulation Counter : 199, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:04 PM]Simulation Counter : 200, Last winner cat had: 14 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:11 PM]Simulation Counter : 201, Last winner cat had: 12 points! Last winner dog had: 10.5 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:18 PM]Simulation Counter : 202, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:25 PM]Simulation Counter : 203, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:32 PM]Simulation Counter : 204, Last winner cat had: 12 points! Last winner dog had: 20.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:39 PM]Simulation Counter : 205, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:46 PM]Simulation Counter : 206, Last winner cat had: 12 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:41:53 PM]Simulation Counter : 207, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:00 PM]Simulation Counter : 208, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:07 PM]Simulation Counter : 209, Last winner cat had: 10 points! Last winner dog had: 10.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:14 PM]Simulation Counter : 210, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:21 PM]Simulation Counter : 211, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:28 PM]Simulation Counter : 212, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:35 PM]Simulation Counter : 213, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:42 PM]Simulation Counter : 214, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:49 PM]Simulation Counter : 215, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:42:56 PM]Simulation Counter : 216, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:03 PM]Simulation Counter : 217, Last winner cat had: 10 points! Last winner dog had: 15.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:10 PM]Simulation Counter : 218, Last winner cat had: 12 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:17 PM]Simulation Counter : 219, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:24 PM]Simulation Counter : 220, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:31 PM]Simulation Counter : 221, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:38 PM]Simulation Counter : 222, Last winner cat had: 10 points! Last winner dog had: 20 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:45 PM]Simulation Counter : 223, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:52 PM]Simulation Counter : 224, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:43:59 PM]Simulation Counter : 225, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:06 PM]Simulation Counter : 226, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:13 PM]Simulation Counter : 227, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:20 PM]Simulation Counter : 228, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:27 PM]Simulation Counter : 229, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:34 PM]Simulation Counter : 230, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:41 PM]Simulation Counter : 231, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:48 PM]Simulation Counter : 232, Last winner cat had: 12 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:44:55 PM]Simulation Counter : 233, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:02 PM]Simulation Counter : 234, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:09 PM]Simulation Counter : 235, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:16 PM]Simulation Counter : 236, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:23 PM]Simulation Counter : 237, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:30 PM]Simulation Counter : 238, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:37 PM]Simulation Counter : 239, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:44 PM]Simulation Counter : 240, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:51 PM]Simulation Counter : 241, Last winner cat had: 10 points! Last winner dog had: 15.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:45:58 PM]Simulation Counter : 242, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:05 PM]Simulation Counter : 243, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:12 PM]Simulation Counter : 244, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:19 PM]Simulation Counter : 245, Last winner cat had: 10 points! Last winner dog had: 10.3 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:26 PM]Simulation Counter : 246, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:33 PM]Simulation Counter : 247, Last winner cat had: 14 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:40 PM]Simulation Counter : 248, Last winner cat had: 12 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:47 PM]Simulation Counter : 249, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:46:54 PM]Simulation Counter : 250, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:47:01 PM]Simulation Counter : 251, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:47:08 PM]Simulation Counter : 252, Last winner cat had: 10 points! Last winner dog had: 15.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:47:15 PM]Simulation Counter : 253, Last winner cat had: 10 points! Last winner dog had: 15 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:47:22 PM]Simulation Counter : 254, Last winner cat had: 10 points! Last winner dog had: 20.1 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:47:29 PM]Simulation Counter : 255, Last winner cat had: 10 points! Last winner dog had: 10.4 points!</t>
+  </si>
+  <si>
+    <t>[5/4/2025 8:47:36 PM]Simulation Counter : 256, Last winner cat had: 10 points! Last winner dog had: 10.2 points!</t>
   </si>
 </sst>
 </file>
@@ -4742,15 +5516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76559D-2104-4C42-96BB-D4003E9D0DC2}">
-  <dimension ref="A1:Y786"/>
+  <dimension ref="A1:AJ786"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4760,8 +5534,11 @@
       <c r="Y1" t="s">
         <v>1169</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ1" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4771,8 +5548,11 @@
       <c r="Y2" t="s">
         <v>1171</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ2" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4782,8 +5562,11 @@
       <c r="Y3" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ3" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4793,8 +5576,11 @@
       <c r="Y4" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ4" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4804,8 +5590,11 @@
       <c r="Y5" t="s">
         <v>1174</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ5" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4815,8 +5604,11 @@
       <c r="Y6" t="s">
         <v>1175</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ6" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4826,8 +5618,11 @@
       <c r="Y7" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ7" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4837,8 +5632,11 @@
       <c r="Y8" t="s">
         <v>1177</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ8" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4848,8 +5646,11 @@
       <c r="Y9" t="s">
         <v>1178</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ9" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4859,8 +5660,11 @@
       <c r="Y10" t="s">
         <v>1179</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ10" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4870,8 +5674,11 @@
       <c r="Y11" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ11" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4881,8 +5688,11 @@
       <c r="Y12" t="s">
         <v>1181</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ12" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4892,8 +5702,11 @@
       <c r="Y13" t="s">
         <v>1182</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ13" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4903,8 +5716,11 @@
       <c r="Y14" t="s">
         <v>1183</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ14" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4914,8 +5730,11 @@
       <c r="Y15" t="s">
         <v>1184</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ15" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -4925,8 +5744,11 @@
       <c r="Y16" t="s">
         <v>1185</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ16" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -4936,8 +5758,11 @@
       <c r="Y17" t="s">
         <v>1186</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ17" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -4947,8 +5772,11 @@
       <c r="Y18" t="s">
         <v>1187</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ18" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -4958,8 +5786,11 @@
       <c r="Y19" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ19" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -4969,8 +5800,11 @@
       <c r="Y20" t="s">
         <v>1189</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ20" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -4980,8 +5814,11 @@
       <c r="Y21" t="s">
         <v>1190</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ21" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -4991,8 +5828,11 @@
       <c r="Y22" t="s">
         <v>1191</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ22" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -5002,8 +5842,11 @@
       <c r="Y23" t="s">
         <v>1192</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ23" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -5013,8 +5856,11 @@
       <c r="Y24" t="s">
         <v>1193</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ24" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -5024,8 +5870,11 @@
       <c r="Y25" t="s">
         <v>1194</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ25" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -5035,8 +5884,11 @@
       <c r="Y26" t="s">
         <v>1195</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ26" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -5046,8 +5898,11 @@
       <c r="Y27" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ27" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -5057,8 +5912,11 @@
       <c r="Y28" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ28" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -5068,8 +5926,11 @@
       <c r="Y29" t="s">
         <v>1198</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ29" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -5079,8 +5940,11 @@
       <c r="Y30" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ30" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -5090,8 +5954,11 @@
       <c r="Y31" t="s">
         <v>1200</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ31" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -5101,8 +5968,11 @@
       <c r="Y32" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ32" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -5112,8 +5982,11 @@
       <c r="Y33" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ33" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -5123,8 +5996,11 @@
       <c r="Y34" t="s">
         <v>1203</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ34" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -5134,8 +6010,11 @@
       <c r="Y35" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ35" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -5145,8 +6024,11 @@
       <c r="Y36" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ36" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -5156,8 +6038,11 @@
       <c r="Y37" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ37" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -5167,8 +6052,11 @@
       <c r="Y38" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ38" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -5178,8 +6066,11 @@
       <c r="Y39" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ39" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -5189,8 +6080,11 @@
       <c r="Y40" t="s">
         <v>1209</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ40" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -5200,8 +6094,11 @@
       <c r="Y41" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ41" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -5211,8 +6108,11 @@
       <c r="Y42" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ42" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -5222,8 +6122,11 @@
       <c r="Y43" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ43" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -5233,8 +6136,11 @@
       <c r="Y44" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ44" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -5244,8 +6150,11 @@
       <c r="Y45" t="s">
         <v>1214</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ45" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -5255,8 +6164,11 @@
       <c r="Y46" t="s">
         <v>1215</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ46" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -5266,8 +6178,11 @@
       <c r="Y47" t="s">
         <v>1216</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ47" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -5277,8 +6192,11 @@
       <c r="Y48" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ48" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -5288,8 +6206,11 @@
       <c r="Y49" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ49" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -5299,8 +6220,11 @@
       <c r="Y50" t="s">
         <v>1219</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ50" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -5310,8 +6234,11 @@
       <c r="Y51" t="s">
         <v>1220</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ51" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -5321,8 +6248,11 @@
       <c r="Y52" t="s">
         <v>1221</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ52" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -5332,8 +6262,11 @@
       <c r="Y53" t="s">
         <v>1222</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ53" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -5343,8 +6276,11 @@
       <c r="Y54" t="s">
         <v>1223</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ54" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -5354,8 +6290,11 @@
       <c r="Y55" t="s">
         <v>1224</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ55" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -5365,8 +6304,11 @@
       <c r="Y56" t="s">
         <v>1225</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ56" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -5376,8 +6318,11 @@
       <c r="Y57" t="s">
         <v>1226</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ57" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -5387,8 +6332,11 @@
       <c r="Y58" t="s">
         <v>1227</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ58" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -5398,8 +6346,11 @@
       <c r="Y59" t="s">
         <v>1228</v>
       </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ59" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -5409,8 +6360,11 @@
       <c r="Y60" t="s">
         <v>1229</v>
       </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ60" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -5420,8 +6374,11 @@
       <c r="Y61" t="s">
         <v>1230</v>
       </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ61" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -5431,8 +6388,11 @@
       <c r="Y62" t="s">
         <v>1231</v>
       </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ62" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -5442,8 +6402,11 @@
       <c r="Y63" t="s">
         <v>1232</v>
       </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ63" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -5453,8 +6416,11 @@
       <c r="Y64" t="s">
         <v>1233</v>
       </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ64" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -5464,8 +6430,11 @@
       <c r="Y65" t="s">
         <v>1234</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ65" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="66" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -5475,8 +6444,11 @@
       <c r="Y66" t="s">
         <v>1235</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ66" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="67" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -5486,8 +6458,11 @@
       <c r="Y67" t="s">
         <v>1236</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ67" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="68" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -5497,8 +6472,11 @@
       <c r="Y68" t="s">
         <v>1237</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ68" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="69" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -5508,8 +6486,11 @@
       <c r="Y69" t="s">
         <v>1238</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ69" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="70" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -5519,8 +6500,11 @@
       <c r="Y70" t="s">
         <v>1239</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ70" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="71" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -5530,8 +6514,11 @@
       <c r="Y71" t="s">
         <v>1240</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ71" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -5541,8 +6528,11 @@
       <c r="Y72" t="s">
         <v>1241</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ72" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="73" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -5552,8 +6542,11 @@
       <c r="Y73" t="s">
         <v>1242</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ73" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="74" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -5563,8 +6556,11 @@
       <c r="Y74" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ74" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="75" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -5574,8 +6570,11 @@
       <c r="Y75" t="s">
         <v>1244</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ75" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="76" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -5585,8 +6584,11 @@
       <c r="Y76" t="s">
         <v>1245</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ76" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="77" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -5596,8 +6598,11 @@
       <c r="Y77" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ77" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="78" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -5607,8 +6612,11 @@
       <c r="Y78" t="s">
         <v>1247</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ78" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="79" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -5618,8 +6626,11 @@
       <c r="Y79" t="s">
         <v>1248</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ79" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="80" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -5629,8 +6640,11 @@
       <c r="Y80" t="s">
         <v>1249</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ80" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="81" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -5640,8 +6654,11 @@
       <c r="Y81" t="s">
         <v>1250</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ81" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="82" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -5651,8 +6668,11 @@
       <c r="Y82" t="s">
         <v>1251</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ82" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="83" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -5662,8 +6682,11 @@
       <c r="Y83" t="s">
         <v>1252</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ83" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="84" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -5673,8 +6696,11 @@
       <c r="Y84" t="s">
         <v>1253</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ84" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="85" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -5684,8 +6710,11 @@
       <c r="Y85" t="s">
         <v>1254</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ85" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="86" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -5695,8 +6724,11 @@
       <c r="Y86" t="s">
         <v>1255</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ86" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="87" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -5706,8 +6738,11 @@
       <c r="Y87" t="s">
         <v>1256</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ87" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="88" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -5717,8 +6752,11 @@
       <c r="Y88" t="s">
         <v>1257</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ88" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="89" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -5728,8 +6766,11 @@
       <c r="Y89" t="s">
         <v>1258</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ89" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="90" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -5739,8 +6780,11 @@
       <c r="Y90" t="s">
         <v>1259</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ90" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="91" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -5750,8 +6794,11 @@
       <c r="Y91" t="s">
         <v>1260</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ91" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="92" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -5761,8 +6808,11 @@
       <c r="Y92" t="s">
         <v>1261</v>
       </c>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ92" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="93" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -5772,8 +6822,11 @@
       <c r="Y93" t="s">
         <v>1262</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ93" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="94" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -5783,8 +6836,11 @@
       <c r="Y94" t="s">
         <v>1263</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ94" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="95" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -5794,8 +6850,11 @@
       <c r="Y95" t="s">
         <v>1264</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ95" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="96" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -5805,8 +6864,11 @@
       <c r="Y96" t="s">
         <v>1265</v>
       </c>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ96" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="97" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -5816,8 +6878,11 @@
       <c r="Y97" t="s">
         <v>1266</v>
       </c>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ97" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="98" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -5827,8 +6892,11 @@
       <c r="Y98" t="s">
         <v>1267</v>
       </c>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ98" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="99" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -5838,8 +6906,11 @@
       <c r="Y99" t="s">
         <v>1268</v>
       </c>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ99" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="100" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -5849,8 +6920,11 @@
       <c r="Y100" t="s">
         <v>1269</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ100" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -5860,8 +6934,11 @@
       <c r="Y101" t="s">
         <v>1270</v>
       </c>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ101" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="102" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -5871,8 +6948,11 @@
       <c r="Y102" t="s">
         <v>1271</v>
       </c>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ102" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="103" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -5882,8 +6962,11 @@
       <c r="Y103" t="s">
         <v>1272</v>
       </c>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ103" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -5893,8 +6976,11 @@
       <c r="Y104" t="s">
         <v>1273</v>
       </c>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ104" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="105" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -5904,8 +6990,11 @@
       <c r="Y105" t="s">
         <v>1274</v>
       </c>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ105" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="106" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -5915,8 +7004,11 @@
       <c r="Y106" t="s">
         <v>1275</v>
       </c>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ106" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="107" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -5926,8 +7018,11 @@
       <c r="Y107" t="s">
         <v>1276</v>
       </c>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ107" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="108" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -5937,8 +7032,11 @@
       <c r="Y108" t="s">
         <v>1277</v>
       </c>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ108" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="109" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -5948,8 +7046,11 @@
       <c r="Y109" t="s">
         <v>1278</v>
       </c>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ109" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="110" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -5959,8 +7060,11 @@
       <c r="Y110" t="s">
         <v>1279</v>
       </c>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ110" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="111" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -5970,8 +7074,11 @@
       <c r="Y111" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ111" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="112" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -5981,8 +7088,11 @@
       <c r="Y112" t="s">
         <v>1281</v>
       </c>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ112" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="113" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -5992,8 +7102,11 @@
       <c r="Y113" t="s">
         <v>1282</v>
       </c>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ113" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="114" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -6003,8 +7116,11 @@
       <c r="Y114" t="s">
         <v>1283</v>
       </c>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ114" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="115" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -6014,8 +7130,11 @@
       <c r="Y115" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ115" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="116" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -6025,8 +7144,11 @@
       <c r="Y116" t="s">
         <v>1285</v>
       </c>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ116" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="117" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -6036,8 +7158,11 @@
       <c r="Y117" t="s">
         <v>1286</v>
       </c>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ117" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="118" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -6047,8 +7172,11 @@
       <c r="Y118" t="s">
         <v>1287</v>
       </c>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ118" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="119" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -6058,8 +7186,11 @@
       <c r="Y119" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ119" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="120" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -6069,8 +7200,11 @@
       <c r="Y120" t="s">
         <v>1289</v>
       </c>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ120" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="121" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -6080,8 +7214,11 @@
       <c r="Y121" t="s">
         <v>1290</v>
       </c>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ121" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="122" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -6091,8 +7228,11 @@
       <c r="Y122" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ122" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="123" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -6102,8 +7242,11 @@
       <c r="Y123" t="s">
         <v>1292</v>
       </c>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ123" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="124" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -6113,8 +7256,11 @@
       <c r="Y124" t="s">
         <v>1293</v>
       </c>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ124" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="125" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -6124,8 +7270,11 @@
       <c r="Y125" t="s">
         <v>1294</v>
       </c>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ125" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="126" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -6135,8 +7284,11 @@
       <c r="Y126" t="s">
         <v>1295</v>
       </c>
-    </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ126" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="127" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -6146,8 +7298,11 @@
       <c r="Y127" t="s">
         <v>1296</v>
       </c>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ127" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="128" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -6157,8 +7312,11 @@
       <c r="Y128" t="s">
         <v>1297</v>
       </c>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ128" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="129" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -6168,8 +7326,11 @@
       <c r="Y129" t="s">
         <v>1298</v>
       </c>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ129" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="130" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -6179,8 +7340,11 @@
       <c r="Y130" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ130" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="131" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -6190,8 +7354,11 @@
       <c r="Y131" t="s">
         <v>1300</v>
       </c>
-    </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ131" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="132" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -6201,8 +7368,11 @@
       <c r="Y132" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ132" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="133" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -6212,8 +7382,11 @@
       <c r="Y133" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ133" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="134" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -6223,8 +7396,11 @@
       <c r="Y134" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ134" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="135" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -6234,8 +7410,11 @@
       <c r="Y135" t="s">
         <v>1304</v>
       </c>
-    </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ135" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="136" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -6245,8 +7424,11 @@
       <c r="Y136" t="s">
         <v>1305</v>
       </c>
-    </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ136" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="137" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -6256,8 +7438,11 @@
       <c r="Y137" t="s">
         <v>1306</v>
       </c>
-    </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ137" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="138" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -6267,8 +7452,11 @@
       <c r="Y138" t="s">
         <v>1307</v>
       </c>
-    </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ138" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="139" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -6278,8 +7466,11 @@
       <c r="Y139" t="s">
         <v>1308</v>
       </c>
-    </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ139" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="140" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -6289,8 +7480,11 @@
       <c r="Y140" t="s">
         <v>1309</v>
       </c>
-    </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ140" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="141" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -6300,8 +7494,11 @@
       <c r="Y141" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ141" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="142" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -6311,8 +7508,11 @@
       <c r="Y142" t="s">
         <v>1311</v>
       </c>
-    </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ142" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="143" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -6322,8 +7522,11 @@
       <c r="Y143" t="s">
         <v>1312</v>
       </c>
-    </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ143" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="144" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -6333,8 +7536,11 @@
       <c r="Y144" t="s">
         <v>1313</v>
       </c>
-    </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ144" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="145" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -6344,8 +7550,11 @@
       <c r="Y145" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ145" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="146" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -6355,8 +7564,11 @@
       <c r="Y146" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ146" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="147" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -6366,8 +7578,11 @@
       <c r="Y147" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ147" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="148" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -6377,8 +7592,11 @@
       <c r="Y148" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ148" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="149" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -6388,8 +7606,11 @@
       <c r="Y149" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ149" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="150" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -6399,8 +7620,11 @@
       <c r="Y150" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ150" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="151" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -6410,8 +7634,11 @@
       <c r="Y151" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ151" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="152" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -6421,8 +7648,11 @@
       <c r="Y152" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ152" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="153" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -6432,8 +7662,11 @@
       <c r="Y153" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ153" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="154" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -6443,8 +7676,11 @@
       <c r="Y154" t="s">
         <v>1323</v>
       </c>
-    </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ154" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="155" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -6454,8 +7690,11 @@
       <c r="Y155" t="s">
         <v>1324</v>
       </c>
-    </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ155" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="156" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -6465,8 +7704,11 @@
       <c r="Y156" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ156" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="157" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -6476,8 +7718,11 @@
       <c r="Y157" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ157" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="158" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -6487,8 +7732,11 @@
       <c r="Y158" t="s">
         <v>1327</v>
       </c>
-    </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ158" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="159" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -6498,8 +7746,11 @@
       <c r="Y159" t="s">
         <v>1328</v>
       </c>
-    </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ159" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="160" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -6509,8 +7760,11 @@
       <c r="Y160" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ160" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="161" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -6520,8 +7774,11 @@
       <c r="Y161" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ161" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="162" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -6531,8 +7788,11 @@
       <c r="Y162" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ162" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="163" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -6542,8 +7802,11 @@
       <c r="Y163" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ163" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="164" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -6553,8 +7816,11 @@
       <c r="Y164" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ164" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="165" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -6564,8 +7830,11 @@
       <c r="Y165" t="s">
         <v>1334</v>
       </c>
-    </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ165" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="166" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -6575,8 +7844,11 @@
       <c r="Y166" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ166" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="167" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -6586,8 +7858,11 @@
       <c r="Y167" t="s">
         <v>1336</v>
       </c>
-    </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ167" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="168" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -6597,8 +7872,11 @@
       <c r="Y168" t="s">
         <v>1337</v>
       </c>
-    </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ168" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="169" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -6608,8 +7886,11 @@
       <c r="Y169" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ169" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="170" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -6619,8 +7900,11 @@
       <c r="Y170" t="s">
         <v>1339</v>
       </c>
-    </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ170" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="171" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -6630,8 +7914,11 @@
       <c r="Y171" t="s">
         <v>1340</v>
       </c>
-    </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ171" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="172" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -6641,8 +7928,11 @@
       <c r="Y172" t="s">
         <v>1341</v>
       </c>
-    </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ172" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="173" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -6652,8 +7942,11 @@
       <c r="Y173" t="s">
         <v>1342</v>
       </c>
-    </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ173" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="174" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -6663,8 +7956,11 @@
       <c r="Y174" t="s">
         <v>1343</v>
       </c>
-    </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ174" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="175" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -6674,8 +7970,11 @@
       <c r="Y175" t="s">
         <v>1344</v>
       </c>
-    </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ175" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="176" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -6685,8 +7984,11 @@
       <c r="Y176" t="s">
         <v>1345</v>
       </c>
-    </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ176" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="177" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -6696,8 +7998,11 @@
       <c r="Y177" t="s">
         <v>1346</v>
       </c>
-    </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ177" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="178" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -6707,8 +8012,11 @@
       <c r="Y178" t="s">
         <v>1347</v>
       </c>
-    </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ178" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="179" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -6718,8 +8026,11 @@
       <c r="Y179" t="s">
         <v>1348</v>
       </c>
-    </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ179" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="180" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -6729,8 +8040,11 @@
       <c r="Y180" t="s">
         <v>1349</v>
       </c>
-    </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ180" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="181" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -6740,8 +8054,11 @@
       <c r="Y181" t="s">
         <v>1350</v>
       </c>
-    </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ181" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="182" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -6751,8 +8068,11 @@
       <c r="Y182" t="s">
         <v>1351</v>
       </c>
-    </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ182" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="183" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -6762,8 +8082,11 @@
       <c r="Y183" t="s">
         <v>1352</v>
       </c>
-    </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ183" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="184" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -6773,8 +8096,11 @@
       <c r="Y184" t="s">
         <v>1353</v>
       </c>
-    </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ184" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="185" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -6784,8 +8110,11 @@
       <c r="Y185" t="s">
         <v>1354</v>
       </c>
-    </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ185" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="186" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -6795,8 +8124,11 @@
       <c r="Y186" t="s">
         <v>1355</v>
       </c>
-    </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ186" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="187" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -6806,8 +8138,11 @@
       <c r="Y187" t="s">
         <v>1356</v>
       </c>
-    </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ187" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="188" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -6817,8 +8152,11 @@
       <c r="Y188" t="s">
         <v>1357</v>
       </c>
-    </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ188" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="189" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -6828,8 +8166,11 @@
       <c r="Y189" t="s">
         <v>1358</v>
       </c>
-    </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ189" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="190" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -6839,8 +8180,11 @@
       <c r="Y190" t="s">
         <v>1359</v>
       </c>
-    </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ190" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="191" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -6850,8 +8194,11 @@
       <c r="Y191" t="s">
         <v>1360</v>
       </c>
-    </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ191" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="192" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -6861,8 +8208,11 @@
       <c r="Y192" t="s">
         <v>1361</v>
       </c>
-    </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ192" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="193" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -6872,8 +8222,11 @@
       <c r="Y193" t="s">
         <v>1362</v>
       </c>
-    </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ193" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="194" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -6883,8 +8236,11 @@
       <c r="Y194" t="s">
         <v>1363</v>
       </c>
-    </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ194" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="195" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -6894,8 +8250,11 @@
       <c r="Y195" t="s">
         <v>1364</v>
       </c>
-    </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ195" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="196" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -6905,8 +8264,11 @@
       <c r="Y196" t="s">
         <v>1365</v>
       </c>
-    </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ196" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="197" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -6916,8 +8278,11 @@
       <c r="Y197" t="s">
         <v>1366</v>
       </c>
-    </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ197" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="198" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -6927,8 +8292,11 @@
       <c r="Y198" t="s">
         <v>1367</v>
       </c>
-    </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ198" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="199" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -6938,8 +8306,11 @@
       <c r="Y199" t="s">
         <v>1368</v>
       </c>
-    </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ199" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="200" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -6949,8 +8320,11 @@
       <c r="Y200" t="s">
         <v>1369</v>
       </c>
-    </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ200" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="201" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -6960,8 +8334,11 @@
       <c r="Y201" t="s">
         <v>1370</v>
       </c>
-    </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ201" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="202" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -6971,8 +8348,11 @@
       <c r="Y202" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ202" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="203" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -6982,8 +8362,11 @@
       <c r="Y203" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ203" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="204" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -6993,8 +8376,11 @@
       <c r="Y204" t="s">
         <v>1373</v>
       </c>
-    </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ204" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="205" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -7004,8 +8390,11 @@
       <c r="Y205" t="s">
         <v>1374</v>
       </c>
-    </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ205" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="206" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -7015,8 +8404,11 @@
       <c r="Y206" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ206" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="207" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -7026,8 +8418,11 @@
       <c r="Y207" t="s">
         <v>1376</v>
       </c>
-    </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ207" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="208" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -7037,8 +8432,11 @@
       <c r="Y208" t="s">
         <v>1377</v>
       </c>
-    </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ208" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="209" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -7048,8 +8446,11 @@
       <c r="Y209" t="s">
         <v>1378</v>
       </c>
-    </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ209" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="210" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -7059,8 +8460,11 @@
       <c r="Y210" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ210" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="211" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -7070,8 +8474,11 @@
       <c r="Y211" t="s">
         <v>1380</v>
       </c>
-    </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ211" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="212" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -7081,8 +8488,11 @@
       <c r="Y212" t="s">
         <v>1381</v>
       </c>
-    </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ212" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="213" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -7092,8 +8502,11 @@
       <c r="Y213" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ213" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="214" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -7103,8 +8516,11 @@
       <c r="Y214" t="s">
         <v>1383</v>
       </c>
-    </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ214" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="215" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -7114,8 +8530,11 @@
       <c r="Y215" t="s">
         <v>1384</v>
       </c>
-    </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ215" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="216" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -7125,8 +8544,11 @@
       <c r="Y216" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ216" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="217" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -7136,8 +8558,11 @@
       <c r="Y217" t="s">
         <v>1386</v>
       </c>
-    </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ217" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="218" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -7147,8 +8572,11 @@
       <c r="Y218" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ218" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="219" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -7158,8 +8586,11 @@
       <c r="Y219" t="s">
         <v>1388</v>
       </c>
-    </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ219" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="220" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -7169,8 +8600,11 @@
       <c r="Y220" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ220" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="221" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -7180,8 +8614,11 @@
       <c r="Y221" t="s">
         <v>1390</v>
       </c>
-    </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ221" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="222" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -7191,8 +8628,11 @@
       <c r="Y222" t="s">
         <v>1391</v>
       </c>
-    </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ222" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="223" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -7202,8 +8642,11 @@
       <c r="Y223" t="s">
         <v>1392</v>
       </c>
-    </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ223" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="224" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -7213,8 +8656,11 @@
       <c r="Y224" t="s">
         <v>1393</v>
       </c>
-    </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ224" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="225" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -7224,8 +8670,11 @@
       <c r="Y225" t="s">
         <v>1394</v>
       </c>
-    </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ225" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="226" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -7235,8 +8684,11 @@
       <c r="Y226" t="s">
         <v>1395</v>
       </c>
-    </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ226" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="227" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -7246,8 +8698,11 @@
       <c r="Y227" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ227" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="228" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -7257,8 +8712,11 @@
       <c r="Y228" t="s">
         <v>1397</v>
       </c>
-    </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ228" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="229" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -7268,8 +8726,11 @@
       <c r="Y229" t="s">
         <v>1398</v>
       </c>
-    </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ229" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="230" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -7279,8 +8740,11 @@
       <c r="Y230" t="s">
         <v>1399</v>
       </c>
-    </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ230" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="231" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -7290,8 +8754,11 @@
       <c r="Y231" t="s">
         <v>1400</v>
       </c>
-    </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ231" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="232" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -7301,8 +8768,11 @@
       <c r="Y232" t="s">
         <v>1401</v>
       </c>
-    </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ232" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="233" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -7312,8 +8782,11 @@
       <c r="Y233" t="s">
         <v>1402</v>
       </c>
-    </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ233" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="234" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -7323,8 +8796,11 @@
       <c r="Y234" t="s">
         <v>1403</v>
       </c>
-    </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ234" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="235" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -7334,8 +8810,11 @@
       <c r="Y235" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ235" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="236" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -7345,8 +8824,11 @@
       <c r="Y236" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ236" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="237" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -7356,8 +8838,11 @@
       <c r="Y237" t="s">
         <v>1406</v>
       </c>
-    </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ237" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="238" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -7367,8 +8852,11 @@
       <c r="Y238" t="s">
         <v>1407</v>
       </c>
-    </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ238" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="239" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -7378,8 +8866,11 @@
       <c r="Y239" t="s">
         <v>1408</v>
       </c>
-    </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ239" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="240" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -7389,8 +8880,11 @@
       <c r="Y240" t="s">
         <v>1409</v>
       </c>
-    </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ240" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="241" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -7400,8 +8894,11 @@
       <c r="Y241" t="s">
         <v>1410</v>
       </c>
-    </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ241" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="242" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -7411,8 +8908,11 @@
       <c r="Y242" t="s">
         <v>1411</v>
       </c>
-    </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ242" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="243" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -7422,8 +8922,11 @@
       <c r="Y243" t="s">
         <v>1412</v>
       </c>
-    </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ243" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="244" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -7433,8 +8936,11 @@
       <c r="Y244" t="s">
         <v>1413</v>
       </c>
-    </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ244" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="245" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -7444,8 +8950,11 @@
       <c r="Y245" t="s">
         <v>1414</v>
       </c>
-    </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ245" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="246" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -7455,8 +8964,11 @@
       <c r="Y246" t="s">
         <v>1415</v>
       </c>
-    </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ246" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="247" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -7466,8 +8978,11 @@
       <c r="Y247" t="s">
         <v>1416</v>
       </c>
-    </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ247" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="248" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -7477,8 +8992,11 @@
       <c r="Y248" t="s">
         <v>1417</v>
       </c>
-    </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ248" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="249" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -7488,8 +9006,11 @@
       <c r="Y249" t="s">
         <v>1418</v>
       </c>
-    </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ249" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="250" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -7499,8 +9020,11 @@
       <c r="Y250" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ250" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="251" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -7510,8 +9034,11 @@
       <c r="Y251" t="s">
         <v>1420</v>
       </c>
-    </row>
-    <row r="252" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ251" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="252" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -7521,8 +9048,11 @@
       <c r="Y252" t="s">
         <v>1421</v>
       </c>
-    </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ252" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="253" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -7532,8 +9062,11 @@
       <c r="Y253" t="s">
         <v>1422</v>
       </c>
-    </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ253" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="254" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -7543,8 +9076,11 @@
       <c r="Y254" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ254" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="255" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -7554,8 +9090,11 @@
       <c r="Y255" t="s">
         <v>1424</v>
       </c>
-    </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ255" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="256" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -7565,8 +9104,11 @@
       <c r="Y256" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ256" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="257" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -7576,8 +9118,11 @@
       <c r="Y257" t="s">
         <v>1426</v>
       </c>
-    </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ257" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="258" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -7587,8 +9132,11 @@
       <c r="Y258" t="s">
         <v>1427</v>
       </c>
-    </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AJ258" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="259" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -7599,7 +9147,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -7610,7 +9158,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -7621,7 +9169,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -7632,7 +9180,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -7643,7 +9191,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -7654,7 +9202,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -7665,7 +9213,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -7676,7 +9224,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -7687,7 +9235,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -7698,7 +9246,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -7709,7 +9257,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -7720,7 +9268,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -7731,7 +9279,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>271</v>
       </c>

</xml_diff>